<commit_message>
Deploying to gh-pages from  @ f1537a4d2bc3eab4cb9bd8f47167308c570ee746 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_8-1-1.xlsx
+++ b/assets/excel/2021_8-1-1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24834399-6D65-4625-B399-3D2278393774}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19A5ACE9-0DAD-4B50-9B83-2396A92B7273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{3ED27CCD-7831-47CD-9649-40DDA4FF2B68}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="14010" xr2:uid="{3ED27CCD-7831-47CD-9649-40DDA4FF2B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -91,20 +91,10 @@
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
   </si>
   <si>
-    <r>
-      <t>Tabelle 8.1.1: Bei Bundes- und Landtagswahlen wahlberechtigte Bevölkerung mit Zuwanderungsgeschichte nach Altersgruppen und Geschlecht im Jahr 2019</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <rFont val="NDSFrutiger 55 Roman"/>
-      </rPr>
-      <t>1)</t>
-    </r>
+    <t>2) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes</t>
   </si>
   <si>
-    <t>2) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes</t>
+    <t>Tabelle 8.1.1: Bei Bundes- und Landtagswahlen wahlberechtigte Bevölkerung mit Zuwanderungsgeschichte nach Altersgruppen und Geschlecht</t>
   </si>
 </sst>
 </file>
@@ -117,7 +107,7 @@
     <numFmt numFmtId="166" formatCode="[&lt;5]&quot;-&quot;;[&lt;10]\(0.0\);#\ ###.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,11 +121,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="NDSFrutiger 55 Roman"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
       <name val="NDSFrutiger 55 Roman"/>
     </font>
     <font>
@@ -352,7 +337,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -375,97 +360,97 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -474,52 +459,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -837,6 +822,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F150A0D7-5577-4BEA-A4C0-1815A7A8D6E5}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:L190"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -871,7 +857,7 @@
     </row>
     <row r="4" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2294,7 +2280,7 @@
     </row>
     <row r="59" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>

</xml_diff>